<commit_message>
icons sin internet, select2, precios con decimales, avance del pdf del comprobante
</commit_message>
<xml_diff>
--- a/src/archives/productos.xlsx
+++ b/src/archives/productos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\yoxer\PROYECTOS DESARROLLADOS\EYVI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\yoxer\PROYECTOS DESARROLLADOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5934050-6409-47E4-9E89-36F4CED79C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863316CA-4C81-41B6-826F-9A32317ED583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5D8917FB-2979-4D69-ACF6-67AA3D6F31EF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>nombre</t>
   </si>
@@ -44,36 +44,15 @@
     <t>marca</t>
   </si>
   <si>
-    <t>detalle</t>
-  </si>
-  <si>
-    <t>precio</t>
-  </si>
-  <si>
     <t>stock</t>
   </si>
   <si>
     <t>producto 1</t>
   </si>
   <si>
-    <t>detalle 1</t>
-  </si>
-  <si>
     <t>producto 2</t>
   </si>
   <si>
-    <t>detalle 2</t>
-  </si>
-  <si>
-    <t>https://imgs.search.brave.com/U-VzSQ7xPJO8mW5dZ8O8-ItXIbMAKCwQgrk4OpeV6uc/rs:fit:860:0:0:0/g:ce/aHR0cHM6Ly9tZWRp/YS5nZXR0eWltYWdl/cy5jb20vaWQvMTcw/OTYxODY3L2VzL2Zv/dG8vdHJhYmFqYWRv/cmVzLWRlLWxhLWNv/bnN0cnVjY2klQzMl/QjNuLWVuLXNpdGlv/LWRlLWNvbnN0cnVj/Y2klQzMlQjNuLmpw/Zz9zPTYxMng2MTIm/dz0wJms9MjAmYz11/d2RQblZKSVpfbkNz/WmZDOEg5VVlTaDJJ/SUN3MkIwR0Q0R0U1/cDRyZWlZPQ</t>
-  </si>
-  <si>
-    <t>https://imgs.search.brave.com/VDA61APxJpAi9T8D7UaimiEEJPBe9VUv3cppdFrz2cw/rs:fit:860:0:0:0/g:ce/aHR0cHM6Ly9tZWRp/YS5nZXR0eWltYWdl/cy5jb20vaWQvMTgz/ODgyNTUyL2VzL2Zv/dG8vbWF0ZXJpYWwt/ZGUtY29uc3RydWNj/aSVDMyVCM24uanBn/P3M9NjEyeDYxMiZ3/PTAmaz0yMCZjPWR1/d2E5YmdjY2tMcExx/bF8xZVR2Ym9PSGdk/TjNKMnhhZHJRdWtr/bWpwdms9</t>
-  </si>
-  <si>
-    <t>imagen</t>
-  </si>
-  <si>
     <t>marca 1</t>
   </si>
   <si>
@@ -98,15 +77,6 @@
     <t>marca 5</t>
   </si>
   <si>
-    <t>detalle 3</t>
-  </si>
-  <si>
-    <t>detalle 4</t>
-  </si>
-  <si>
-    <t>detalle 5</t>
-  </si>
-  <si>
     <t>categoría</t>
   </si>
   <si>
@@ -158,61 +128,19 @@
     <t>marca 12</t>
   </si>
   <si>
-    <t>detalle 6</t>
-  </si>
-  <si>
-    <t>detalle 7</t>
-  </si>
-  <si>
-    <t>detalle 8</t>
-  </si>
-  <si>
-    <t>detalle 9</t>
-  </si>
-  <si>
-    <t>detalle 10</t>
-  </si>
-  <si>
-    <t>detalle 11</t>
-  </si>
-  <si>
-    <t>detalle 12</t>
-  </si>
-  <si>
-    <t>https://imgs.search.brave.com/sxqXrfFjiunl_3jhKL9sMdl7ib4I1EasolzJm1qurVA/rs:fit:860:0:0:0/g:ce/aHR0cHM6Ly9tZWRp/YS5pc3RvY2twaG90/by5jb20vaWQvNTIx/ODI3ODQ3L2VzL2Zv/dG8vc29sZGFkdXJh/LWRlLWFjZXJvLmpw/Zz9zPTYxMng2MTIm/dz0wJms9MjAmYz12/RGZWM2d4TTJGbWRn/eHpGMHR1dTFaR19Z/WUlnQVRRc3ZKUktY/SzlDS1dJPQ</t>
-  </si>
-  <si>
-    <t>https://imgs.search.brave.com/JsDwc31F_4iU0MQF98ZJ3ebX2cm74oftJjM8VELlHvA/rs:fit:860:0:0:0/g:ce/aHR0cHM6Ly9jZG4u/cGl4YWJheS5jb20v/cGhvdG8vMjAxOC8w/NS8xMS8xMS8yOS9j/b25zdHJ1Y3Rpb24t/MzM5MDMxOF9fMzQw/LmpwZw</t>
-  </si>
-  <si>
-    <t>https://imgs.search.brave.com/f9e1tQBjmPtMZ8ii4HX5u0a27lAQb6ov37oYGpTIHxk/rs:fit:860:0:0:0/g:ce/aHR0cHM6Ly9tZWRp/YS5nZXR0eWltYWdl/cy5jb20vaWQvMTY4/MzYyNzI4L2VzL2Zv/dG8vaGVycmFtaWVu/dGFzLmpwZz9zPTYx/Mng2MTImdz0wJms9/MjAmYz03aU8tU2hN/TlFZTGhJMUtmazhT/OFROdHFfVUtzZlll/YkkzbDRHczF2OExz/PQ</t>
-  </si>
-  <si>
-    <t>https://imgs.search.brave.com/CjOvPgcZT3SjV8Jkg5YHdsB3Q6j6LiLEQjeWRDVYqes/rs:fit:860:0:0:0/g:ce/aHR0cHM6Ly9tZWRp/YS5pc3RvY2twaG90/by5jb20vaWQvNDg0/OTMwMjU4L2VzL2Zv/dG8vaGVycmFtaWVu/dGFzLmpwZz9zPTYx/Mng2MTImdz0wJms9/MjAmYz1hWktaa1Jx/d1RlSUlLNmtLampQ/YjVVR0R4SXdaNnRR/TXREaUpoM0pwTklV/PQ</t>
-  </si>
-  <si>
-    <t>https://imgs.search.brave.com/Ap4HESQH1mDRdCZvH0t6blNj1Q8emwbJj6EjzQF-Fpw/rs:fit:860:0:0:0/g:ce/aHR0cHM6Ly9tZWRp/YS5pc3RvY2twaG90/by5jb20vaWQvNDY1/MTM3MjMwL2VzL2Zv/dG8vY2FqYS1kZS1o/ZXJyYW1pZW50YXMu/anBnP3M9NjEyeDYx/MiZ3PTAmaz0yMCZj/PVNXWDhGMDU1QTFz/ZFlDM0hMX2xINS1W/Ui1BaGpTVnRpbDZR/NFpXa25VcTA9</t>
-  </si>
-  <si>
-    <t>https://imgs.search.brave.com/U46POEUf-Bx1KfioU3QhGXjp84y7SPZ3DRxiEPAIBqE/rs:fit:860:0:0:0/g:ce/aHR0cHM6Ly9odHRw/Mi5tbHN0YXRpYy5j/b20vRF9OUV82MTEy/NzEtTUxBNzU5NjU5/NzE0ODhfMDUyMDI0/LVYud2VicA</t>
-  </si>
-  <si>
-    <t>https://imgs.search.brave.com/18F-d7IUPP-Ud9lv2O2DnzGAI6goayYVTPYsU0sADvg/rs:fit:860:0:0:0/g:ce/aHR0cHM6Ly9odHRw/Mi5tbHN0YXRpYy5j/b20vRF9OUV82NjA3/MzQtTUxBNzU5NDky/Nzg3NzBfMDUyMDI0/LVYud2VicA</t>
-  </si>
-  <si>
-    <t>https://imgs.search.brave.com/RP3OGEQd_S91phuDnh2pZp7a4CMZ7yRA-GJYGcd6efY/rs:fit:860:0:0:0/g:ce/aHR0cHM6Ly9odHRw/Mi5tbHN0YXRpYy5j/b20vRF9OUV84ODAw/NjMtTUxBNzYxNDA1/OTg5MDVfMDUyMDI0/LVYud2VicA</t>
-  </si>
-  <si>
-    <t>https://imgs.search.brave.com/rTn2imWOp5mAKdxt7SRUj7W4yAAyApnyy0vylJBUHJY/rs:fit:860:0:0:0/g:ce/aHR0cHM6Ly9odHRw/Mi5tbHN0YXRpYy5j/b20vRF9OUV83MjQ3/NjUtTUxBNzU5NjU1/NDE3MzZfMDUyMDI0/LVYud2VicA</t>
-  </si>
-  <si>
-    <t>https://imgs.search.brave.com/ofJH6DYxBnnRMxJpVs_zr6S6D-IZ10vBNCNf2prWgLE/rs:fit:860:0:0:0/g:ce/aHR0cHM6Ly9tZWRp/YS5nZXR0eWltYWdl/cy5jb20vaWQvMTQw/NDc3NDYzOS9lcy9m/b3RvL211Y2hvcy10/YWxhZHJvcy1lbCVD/MyVBOWN0cmljb3Mt/ZW4tZWwtZXN0YW50/ZS5qcGc_cz02MTJ4/NjEyJnc9MCZrPTIw/JmM9VzNXaUNaaC1O/VlM4RE9ZS0puRGpY/azk1MmFkZUMzUkst/ejlqMlRxQ1ZrQT0</t>
+    <t>precio(u)</t>
+  </si>
+  <si>
+    <t>precio(m)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="&quot;S/&quot;\ #,##0.00"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -236,7 +164,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -274,26 +202,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -302,13 +215,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -643,20 +557,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DFC6074-C2AC-40C0-9B52-2D18DFD63CE8}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD13"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="11.5546875" style="2"/>
-    <col min="5" max="6" width="11.5546875" style="5"/>
-    <col min="7" max="7" width="11.5546875" style="2"/>
+    <col min="1" max="3" width="11.5546875" style="2"/>
+    <col min="4" max="5" width="11.5546875" style="7"/>
+    <col min="6" max="6" width="11.5546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -664,295 +578,256 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="7">
+        <v>1299.99</v>
+      </c>
+      <c r="E2" s="7">
+        <v>1099.99</v>
+      </c>
+      <c r="F2" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="7">
+        <v>300</v>
+      </c>
+      <c r="E3" s="7">
+        <v>300</v>
+      </c>
+      <c r="F3" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="7">
+        <v>678</v>
+      </c>
+      <c r="E4" s="7">
+        <v>678</v>
+      </c>
+      <c r="F4" s="4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="7">
+        <v>99</v>
+      </c>
+      <c r="E5" s="7">
+        <v>99</v>
+      </c>
+      <c r="F5" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="7">
+        <v>101</v>
+      </c>
+      <c r="E6" s="7">
+        <v>101</v>
+      </c>
+      <c r="F6" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="C7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="7">
+        <v>10</v>
+      </c>
+      <c r="E7" s="7">
+        <v>10</v>
+      </c>
+      <c r="F7" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="7">
+        <v>50</v>
+      </c>
+      <c r="E8" s="7">
+        <v>50</v>
+      </c>
+      <c r="F8" s="4">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="5">
-        <v>1299</v>
-      </c>
-      <c r="F2" s="5">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="7">
+        <v>15</v>
+      </c>
+      <c r="E9" s="7">
+        <v>15</v>
+      </c>
+      <c r="F9" s="4">
         <v>30</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="5">
-        <v>300</v>
-      </c>
-      <c r="F3" s="5">
-        <v>25</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="2" t="s">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="7">
+        <v>237</v>
+      </c>
+      <c r="E10" s="7">
+        <v>237.25</v>
+      </c>
+      <c r="F10" s="4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="5">
-        <v>678</v>
-      </c>
-      <c r="F4" s="5">
-        <v>40</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="B11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="7">
+        <v>407</v>
+      </c>
+      <c r="E11" s="7">
+        <v>407</v>
+      </c>
+      <c r="F11" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="5">
-        <v>99</v>
-      </c>
-      <c r="F5" s="5">
-        <v>30</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="B12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="D12" s="7">
+        <v>1205</v>
+      </c>
+      <c r="E12" s="7">
+        <v>1205</v>
+      </c>
+      <c r="F12" s="4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="5">
-        <v>101</v>
-      </c>
-      <c r="F6" s="5">
-        <v>30</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="5">
-        <v>10</v>
-      </c>
-      <c r="F7" s="5">
-        <v>30</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="5">
-        <v>50</v>
-      </c>
-      <c r="F8" s="5">
-        <v>11</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="5">
-        <v>15</v>
-      </c>
-      <c r="F9" s="5">
-        <v>30</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="5">
-        <v>237</v>
-      </c>
-      <c r="F10" s="5">
+      <c r="C13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="5">
-        <v>407</v>
-      </c>
-      <c r="F11" s="5">
-        <v>30</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="5">
-        <v>1205</v>
-      </c>
-      <c r="F12" s="5">
-        <v>32</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="5">
-        <v>11</v>
-      </c>
-      <c r="F13" s="5">
+      <c r="D13" s="7">
+        <v>11.5</v>
+      </c>
+      <c r="E13" s="7">
+        <v>10.43</v>
+      </c>
+      <c r="F13" s="4">
         <v>23</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>